<commit_message>
Correciones con lectura de Excel para distribuidos
</commit_message>
<xml_diff>
--- a/Netlist excel/circuito_4.xlsx
+++ b/Netlist excel/circuito_4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cinvestav365-my.sharepoint.com/personal/saul_gonzalez_cinvestav_mx/Documents/Documentos 1/MATLAB/Proyecto Simulador de circuitos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monts\OneDrive\Documentos\Escuela\Cinvestav\Primer Cuatrimestre\RFI\Proyecto\Netlist excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_AD4D2F04E46CFB4ACB3E20592D96C87C693EDF10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BB97FB8-0A3B-47DC-9FC8-D2AE94D02E57}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A0D19D-F6FE-4836-BE02-D7E65546F412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="617" yWindow="3351" windowWidth="24694" windowHeight="13595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7830" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Nombre</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL </t>
+  </si>
+  <si>
+    <t>Operating frequency</t>
   </si>
 </sst>
 </file>
@@ -113,14 +119,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -138,10 +138,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,29 +406,35 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -445,11 +447,17 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>5.0000000000000002E-11</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -462,11 +470,17 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>4.9999999999999998E-8</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -482,9 +496,15 @@
       <c r="E4">
         <v>5</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="H6" s="4"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>